<commit_message>
updated model of MOSFET (terminal and ground)
</commit_message>
<xml_diff>
--- a/motor_control_resources.xlsx
+++ b/motor_control_resources.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1bcb454f33dbfecf/mkn_dieukhiendongco/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\awesome_motor_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1A69BAA-885B-4FF4-9388-BB7F84209D8E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F53C46-9093-4F88-8A71-63EA0C46722F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="online_resources" sheetId="2" r:id="rId2"/>
+    <sheet name="maker" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -896,7 +897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1253,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552C6C56-DD4C-4C20-95F6-70DF4AECDE95}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:C18"/>
+    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1407,4 +1408,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E5F793-729B-4D0C-A183-F57DE517F414}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="55.375" customWidth="1"/>
+    <col min="2" max="2" width="67.75" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="11"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>